<commit_message>
Updated (NEWSITE + CV)
</commit_message>
<xml_diff>
--- a/cv/data/cv_entries.xlsx
+++ b/cv/data/cv_entries.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bttom\OneDrive - FURB\Documentos\GitHub\bttomio.github.io\cv\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D52D699C-AC14-481C-A26E-2F691A539292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C78D102F-67FE-493D-AC38-C3CA6FDC52D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5760" yWindow="456" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>Since Jun/2012</t>
   </si>
   <si>
-    <t>Univ. Grenoble Alpes, France | **[&lt;i class="fab falink0 fa-github"&gt;&lt;/i&gt;](https://github.com/bttomio/UGA_thesisdown)[Thesis repository]{.smaller-font}**</t>
-  </si>
-  <si>
     <t>sharing</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>University of Blumenau, Brazil</t>
+  </si>
+  <si>
+    <t>Univ. Grenoble Alpes, France | **[&lt;i class="fab falink0 fa-github"&gt;&lt;/i&gt;](https://github.com/bttomio/UGA_thesisdown)[&lt;i class="fas fa-folder-open"&gt;&lt;/i&gt;](https://theses.fr/2022GRALE003)**</t>
   </si>
 </sst>
 </file>
@@ -495,7 +495,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,7 +540,7 @@
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="H2" t="s">
         <v>12</v>
@@ -580,7 +580,7 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="H4" t="s">
         <v>12</v>
@@ -597,7 +597,7 @@
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -648,7 +648,7 @@
         <v>26</v>
       </c>
       <c r="E8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -677,44 +677,44 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
+        <v>34</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
         <v>36</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" t="s">
         <v>38</v>
-      </c>
-      <c r="E13" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="D14" t="s">
         <v>42</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>43</v>
-      </c>
-      <c r="E14" t="s">
-        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>